<commit_message>
edit recent app test ,change option structure
</commit_message>
<xml_diff>
--- a/TestSteps/TestSteps diecribe.xlsx
+++ b/TestSteps/TestSteps diecribe.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuia/Desktop/AppiumAutotest/TestSteps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610D1DC0-8B81-0341-95A8-29DCFEE9B83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01886420-1269-294C-924A-70952E7CF10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Wallpaper" sheetId="1" r:id="rId1"/>
     <sheet name="ScreenLock" sheetId="2" r:id="rId2"/>
+    <sheet name="EditLauncher" sheetId="3" r:id="rId3"/>
+    <sheet name="RecentApp" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="67">
   <si>
     <t>Steps</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -215,7 +217,92 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>choose 'update image'</t>
+    <t>edit launcher' button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete 'First App'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>press 'back' button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add 'myviewboard whiteborad' App on hot seat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>find app in All apps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_delete_re-range Apps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>install TestApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>swipe to find TestApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tap TestApp to add on hot seat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uninstall TestApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>End</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open all hot seat apps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tap STB</t>
+  </si>
+  <si>
+    <t>tap STB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open recent app</t>
+  </si>
+  <si>
+    <t>open recent app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear the last open app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear all button</t>
+  </si>
+  <si>
+    <t>clear all button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open show roots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select machine local stroage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select TestPhoto</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -223,7 +310,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,6 +325,49 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -280,20 +410,38 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -610,27 +758,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676EA4B8-998D-1542-982E-CCBA629695EF}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -640,336 +790,489 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
+    <row r="2" spans="1:7" ht="22">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="22">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+    <row r="4" spans="1:7" ht="22">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
+    <row r="5" spans="1:7" ht="22">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
+    <row r="6" spans="1:7" ht="22">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
+    <row r="7" spans="1:7" ht="22">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7">
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
+      <c r="G7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="22">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
+    <row r="9" spans="1:7" ht="22">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F9">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
+    <row r="10" spans="1:7" ht="22">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F10">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
+    <row r="11" spans="1:7" ht="22">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F11">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
+    <row r="12" spans="1:7" ht="22">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F12">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
         <v>11</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
+    <row r="13" spans="1:7" ht="22">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G13" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
+    <row r="14" spans="1:7" ht="22">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="22">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
+      <c r="G15" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="22">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
+    <row r="17" spans="1:8" ht="22">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17">
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
         <v>3</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
+    <row r="18" spans="1:8" ht="22">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F18">
-        <v>4</v>
-      </c>
-      <c r="G18" t="s">
+    </row>
+    <row r="19" spans="1:8" ht="22">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="G19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F19">
+    </row>
+    <row r="20" spans="1:8" ht="22">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G19" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="G20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="22">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
+        <v>7</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="22">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F20">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
+        <v>8</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="22">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <v>9</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="22">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" ht="22">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2">
+        <v>11</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" ht="22">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" ht="22">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2">
+        <v>13</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="22">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2">
+        <v>14</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="B21" t="s">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="22">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2">
+        <v>15</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="22">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F21">
-        <v>7</v>
-      </c>
-      <c r="G21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="F22">
-        <v>8</v>
-      </c>
-      <c r="G22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="F23">
-        <v>9</v>
-      </c>
-      <c r="G23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="F24">
-        <v>10</v>
-      </c>
-      <c r="G24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="F25">
-        <v>11</v>
-      </c>
-      <c r="G25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="F26">
-        <v>12</v>
-      </c>
-      <c r="G26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="F27">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="G28" t="s">
-        <v>32</v>
-      </c>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" ht="22">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="22">
+      <c r="H32" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -977,25 +1280,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1E3124-FA28-6A4B-854D-651EBA37B2FB}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1"/>
+    <sheetView topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -1005,462 +1310,1100 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
+    <row r="2" spans="1:7" ht="22">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:7" ht="22">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+    <row r="4" spans="1:7" ht="22">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
+    <row r="5" spans="1:7" ht="22">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
+    <row r="6" spans="1:7" ht="22">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
+    <row r="7" spans="1:7" ht="22">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="22">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
+    <row r="9" spans="1:7" ht="22">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
+    <row r="10" spans="1:7" ht="22">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
         <v>3</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
+    <row r="11" spans="1:7" ht="22">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F11">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
         <v>4</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
+    <row r="12" spans="1:7" ht="22">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F12">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
         <v>5</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
+    <row r="13" spans="1:7" ht="22">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
         <v>6</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
+    <row r="14" spans="1:7" ht="22">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F14">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
         <v>7</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
+    <row r="15" spans="1:7" ht="22">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F15">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
         <v>8</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
+    <row r="16" spans="1:7" ht="22">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F16">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
         <v>9</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
+    <row r="17" spans="1:7" ht="22">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F17">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
         <v>10</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
+    <row r="18" spans="1:7" ht="22">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F18">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
         <v>11</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
+    <row r="19" spans="1:7" ht="22">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F19">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
+    <row r="20" spans="1:7" ht="22">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G20" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21">
+    <row r="21" spans="1:7" ht="22">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="22">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
       <c r="E22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>1</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23">
+    <row r="23" spans="1:7" ht="22">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24">
+    <row r="24" spans="1:7" ht="22">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F24">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2">
         <v>3</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25">
+    <row r="25" spans="1:7" ht="22">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F25">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2">
         <v>4</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26">
+    <row r="26" spans="1:7" ht="22">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F26">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2">
         <v>5</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27">
+    <row r="27" spans="1:7" ht="22">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F27">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2">
         <v>6</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28">
+    <row r="28" spans="1:7" ht="22">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F28">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2">
         <v>7</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29">
+    <row r="29" spans="1:7" ht="22">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F29">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2">
         <v>8</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30">
+    <row r="30" spans="1:7" ht="22">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G30" t="s">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31">
+    <row r="31" spans="1:7" ht="22">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="22">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="22">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="22">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="22">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="22">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="22">
+      <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6221D9-C25A-7A48-B807-EA75B3523903}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="22">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="22">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="22">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="22">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="22">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="22">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="22">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="22">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="22">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="22">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="22">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="22">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="2">
+        <v>4</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="22">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="22">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="2">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="22">
+      <c r="F18" s="2">
+        <v>7</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="22">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="22">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="22">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="22">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="22">
+      <c r="F23" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F325A5-A711-8349-B968-6B865ABD610A}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="22">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="22">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="22">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="22">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="22">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="22">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="22">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="22">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="22">
+      <c r="E12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="22">
+      <c r="E13" s="7"/>
+      <c r="F13" s="8">
+        <v>2</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22">
+      <c r="F14" s="8">
+        <v>3</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
STB root-view, Freezer , spotlight AT
</commit_message>
<xml_diff>
--- a/TestSteps/TestSteps diecribe.xlsx
+++ b/TestSteps/TestSteps diecribe.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuia/Desktop/AppiumAutotest/TestSteps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636B583A-617F-8A46-BE6D-32F4C8BFD98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D38136E-7643-B744-897B-7B08B4DACFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17440" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="5" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Wallpaper" sheetId="1" r:id="rId1"/>
     <sheet name="ScreenLock" sheetId="2" r:id="rId2"/>
     <sheet name="EditLauncher" sheetId="3" r:id="rId3"/>
     <sheet name="RecentApp" sheetId="4" r:id="rId4"/>
+    <sheet name="STB_root_view" sheetId="5" r:id="rId5"/>
+    <sheet name="STB_Freezer" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="111">
   <si>
     <t>Steps</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -310,11 +312,175 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>input 1111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>check the password remove</t>
+    <t>home button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>back button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open TestApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open STB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tap back button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verify 'text view' label not show</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>homepage button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tap homepage button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>element in all apps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>back to homepage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tap all apps button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>find Testapp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tap TestApp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add apps in shortcut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>initialization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tap allApps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>edit btn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add three element in shortcut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app order in shortcut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove second app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add the second app in shortcut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open second app on shortcut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verify current app is correct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>First Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Second Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Third Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tap allTools</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add two element in shortcut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove first app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add the first app in shortcut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open first app on shortcut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom in &amp; out by button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All tools</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open Freezer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Screenshot compare_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoom in by button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Screenshot compare_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compare different</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoom out by button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoom in by fingers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoom out by fingers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default screen button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom in button first than fingers</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -382,7 +548,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +573,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -422,7 +594,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -454,6 +626,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -772,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676EA4B8-998D-1542-982E-CCBA629695EF}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1301,7 +1479,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1348,9 +1526,6 @@
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="22">
       <c r="A3" s="2">
@@ -1368,9 +1543,6 @@
       <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="4" spans="1:9" ht="22">
       <c r="A4" s="2">
@@ -1416,9 +1588,11 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="22">
@@ -1431,8 +1605,12 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="22">
       <c r="A8" s="2">
@@ -1443,18 +1621,10 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="22">
       <c r="A9" s="2">
@@ -1465,13 +1635,6 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
-        <v>2</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="22">
       <c r="A10" s="2">
@@ -1482,12 +1645,14 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="F10" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="22">
@@ -1501,10 +1666,10 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
-        <v>4</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="22">
@@ -1518,10 +1683,10 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
-        <v>5</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>37</v>
+        <v>3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="22">
@@ -1535,10 +1700,10 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="22">
@@ -1552,10 +1717,10 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
-        <v>7</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="22">
@@ -1569,10 +1734,10 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="22">
@@ -1586,13 +1751,13 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="22">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1603,13 +1768,13 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="22">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1620,13 +1785,13 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2">
-        <v>11</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="22">
+        <v>9</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="22">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1637,13 +1802,13 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="22">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1653,12 +1818,14 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="22">
+      <c r="F20" s="2">
+        <v>11</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="22">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1668,10 +1835,14 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="22">
+      <c r="F21" s="2">
+        <v>12</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="22">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1680,20 +1851,13 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="22">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1703,17 +1867,10 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2">
-        <v>2</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="22">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="22">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1722,15 +1879,17 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="E24" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="F24" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="22">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1741,13 +1900,13 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2">
-        <v>4</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="22">
+        <v>2</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="22">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1758,13 +1917,13 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2">
-        <v>5</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="22">
+        <v>3</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="22">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1775,13 +1934,13 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="22">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1792,13 +1951,13 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
-        <v>7</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="22">
+        <v>5</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="22">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1809,13 +1968,13 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="22">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1825,12 +1984,14 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2">
+        <v>7</v>
+      </c>
       <c r="G30" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="22">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1840,10 +2001,14 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="22">
+      <c r="F31" s="2">
+        <v>8</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="22">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1854,7 +2019,9 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="22">
       <c r="A33" s="2">
@@ -1933,7 +2100,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2250,17 +2417,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F325A5-A711-8349-B968-6B865ABD610A}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22">
@@ -2388,51 +2555,1159 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F9" s="2">
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="22">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="2">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="22">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="22">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="22">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+      <c r="F12" s="2">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="22">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="22">
+      <c r="E15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="22">
+      <c r="E16" s="7"/>
+      <c r="F16" s="8">
+        <v>2</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" ht="22">
+      <c r="F17" s="8">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A8D405-5EA9-F04B-84BA-5031CF24B738}">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="37.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="34.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="E2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="I2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="E3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="F5" s="2">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="2">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8" s="2">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="2">
+        <v>6</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="K10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="E11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="F14" s="2">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="2">
+        <v>3</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="F16" s="2">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11">
+      <c r="F17" s="2">
+        <v>7</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="5:11">
+      <c r="G18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="2">
+        <v>6</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="5:11">
+      <c r="J19" s="2">
+        <v>7</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="5:11">
+      <c r="E20" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="J20" s="2">
+        <v>8</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="5:11">
+      <c r="E21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11">
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J22" s="2">
+        <v>10</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="5:11">
+      <c r="F23" s="2">
+        <v>3</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J23" s="2">
+        <v>11</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="5:11">
+      <c r="F24" s="2">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J24" s="2">
+        <v>12</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="5:11">
+      <c r="F25" s="2">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" s="2">
+        <v>13</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="5:11">
+      <c r="F26" s="2">
+        <v>6</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J26" s="2">
+        <v>14</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="5:11">
+      <c r="F27" s="2">
+        <v>7</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="2">
+        <v>15</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="5:11">
+      <c r="G28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="2">
+        <v>16</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="5:11">
+      <c r="J29" s="2">
+        <v>17</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="5:11">
+      <c r="E30" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J30" s="2">
+        <v>18</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="5:11">
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J31" s="2">
+        <v>19</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="5:11">
+      <c r="F32" s="2">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J32" s="2">
+        <v>20</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11">
+      <c r="F33" s="2">
+        <v>3</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11">
+      <c r="F34" s="2">
+        <v>4</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11">
+      <c r="F35" s="2">
+        <v>5</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11">
+      <c r="F36" s="2">
+        <v>6</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11">
+      <c r="F37" s="2">
+        <v>7</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11">
+      <c r="E40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="5:11">
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="5:11">
+      <c r="F42" s="2">
+        <v>2</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11">
+      <c r="F43" s="2">
+        <v>3</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="5:11">
+      <c r="F44" s="2">
+        <v>4</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="5:11">
+      <c r="F45" s="2">
+        <v>5</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="5:11">
+      <c r="F46" s="2">
+        <v>6</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="5:11">
+      <c r="F47" s="2">
+        <v>7</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="5:11">
+      <c r="F48" s="2">
+        <v>8</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="6:7">
+      <c r="F49" s="2">
+        <v>9</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="6:7">
+      <c r="F50" s="2">
+        <v>10</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="6:7">
+      <c r="F51" s="2">
+        <v>11</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="6:7">
+      <c r="F52" s="2">
+        <v>12</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="6:7">
+      <c r="F53" s="2">
+        <v>13</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="6:7">
+      <c r="F54" s="2">
+        <v>14</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="6:7">
+      <c r="F55" s="2">
+        <v>15</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="6:7">
+      <c r="F56" s="2">
+        <v>16</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="6:7">
+      <c r="F57" s="2">
+        <v>17</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="6:7">
+      <c r="F58" s="2">
+        <v>18</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="6:7">
+      <c r="F59" s="2">
+        <v>19</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="6:7">
+      <c r="F60" s="2">
+        <v>20</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="6:7">
+      <c r="F61" s="2">
+        <v>21</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E70D65-E8B6-1644-86AA-AF9E8E64FD2E}">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="46" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="E2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="2">
+        <v>7</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="2">
+        <v>8</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="F10" s="2">
+        <v>9</v>
+      </c>
       <c r="G10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10" s="2">
+        <v>9</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="22">
-      <c r="E12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="8">
+    <row r="12" spans="1:11">
+      <c r="F12" s="2">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="E15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="2">
         <v>1</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="22">
-      <c r="E13" s="7"/>
-      <c r="F13" s="8">
+      <c r="G15" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="F16" s="2">
         <v>2</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="22">
-      <c r="F14" s="8">
+      <c r="G16" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7">
+      <c r="F17" s="2">
         <v>3</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>62</v>
+      <c r="G17" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7">
+      <c r="F18" s="2">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7">
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7">
+      <c r="F20" s="2">
+        <v>6</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7">
+      <c r="F21" s="2">
+        <v>7</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7">
+      <c r="F22" s="2">
+        <v>8</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7">
+      <c r="F23" s="2">
+        <v>9</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7">
+      <c r="F24" s="2">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7">
+      <c r="F25" s="2">
+        <v>11</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7">
+      <c r="G26" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7">
+      <c r="E28" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7">
+      <c r="F29" s="2">
+        <v>2</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7">
+      <c r="F30" s="2">
+        <v>3</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7">
+      <c r="F31" s="2">
+        <v>4</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7">
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7">
+      <c r="F33" s="2">
+        <v>6</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7">
+      <c r="F34" s="2">
+        <v>7</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7">
+      <c r="F35" s="2">
+        <v>8</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7">
+      <c r="F36" s="2">
+        <v>9</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7">
+      <c r="G37" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
expand add verify steps
</commit_message>
<xml_diff>
--- a/TestSteps/TestSteps diecribe.xlsx
+++ b/TestSteps/TestSteps diecribe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuia/Desktop/AppiumAutotest/TestSteps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BB8B69-670C-4F47-AD34-016D67F530F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31040143-DB64-2B4E-9336-EDA08436AAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" activeTab="7" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" activeTab="8" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Wallpaper" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="STB_Freezer" sheetId="6" r:id="rId6"/>
     <sheet name="STB_spotlight" sheetId="7" r:id="rId7"/>
     <sheet name="STB_stopwatch" sheetId="8" r:id="rId8"/>
+    <sheet name="STB_timer" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="159">
   <si>
     <t>Steps</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -606,6 +607,74 @@
   </si>
   <si>
     <t>expand button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moving</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start and wait bell ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open Timer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting timer_hour '00'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting timer_minute '00'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting timer_second '10'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wait 10 secnonds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>find bell ring image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pause &amp; resume &amp; reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting timer_minute '01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting timer_second '00'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pause button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wait 5 secnonds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resume button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancel button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reset button</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3966,8 +4035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D70AA2A-3BF3-014E-8820-FA500EDCC4CC}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
@@ -4399,15 +4468,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C622E5E-673A-9B43-89DC-D6EC0A744714}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" activeCellId="1" sqref="G28 I25"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="2"/>
     <col min="7" max="7" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -4445,6 +4516,9 @@
       </c>
     </row>
     <row r="2" spans="1:11">
+      <c r="B2" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="E2" s="4" t="s">
         <v>137</v>
       </c>
@@ -4456,6 +4530,505 @@
       </c>
       <c r="I2" s="4" t="s">
         <v>136</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="B6" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="2">
+        <v>7</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="2">
+        <v>8</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="F10" s="2">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="2">
+        <v>9</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="G11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="2">
+        <v>10</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="J12" s="2">
+        <v>11</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="E13" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" s="2">
+        <v>12</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J14" s="2">
+        <v>13</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J15" s="2">
+        <v>14</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="F16" s="2">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11">
+      <c r="F17" s="2">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="5:11">
+      <c r="F18" s="2">
+        <v>6</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="5:11">
+      <c r="F19" s="2">
+        <v>7</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="5:11">
+      <c r="G20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="2">
+        <v>3</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="5:11">
+      <c r="J21" s="2">
+        <v>4</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11">
+      <c r="E22" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="5:11">
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J23" s="2">
+        <v>6</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="5:11">
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J24" s="2">
+        <v>7</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="5:11">
+      <c r="F25" s="2">
+        <v>4</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J25" s="2">
+        <v>8</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="5:11">
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="2">
+        <v>9</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="5:11">
+      <c r="F27" s="2">
+        <v>6</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="2">
+        <v>10</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="5:11">
+      <c r="F28" s="2">
+        <v>7</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J28" s="2">
+        <v>11</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="5:11">
+      <c r="F29" s="2">
+        <v>8</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J29" s="2">
+        <v>12</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="5:11">
+      <c r="F30" s="2">
+        <v>9</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J30" s="2">
+        <v>13</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="5:11">
+      <c r="G31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J31" s="2">
+        <v>14</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="5:11">
+      <c r="J32" s="2">
+        <v>15</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="10:11">
+      <c r="J33" s="2">
+        <v>16</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="10:11">
+      <c r="J34" s="2">
+        <v>17</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="10:11">
+      <c r="K35" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED74A1D-B680-9040-A407-F63FF22649FF}">
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="E2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
@@ -4483,13 +5056,13 @@
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="J4" s="2">
         <v>3</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -4497,13 +5070,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="J5" s="2">
         <v>4</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -4511,13 +5084,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4525,13 +5098,13 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="J7" s="2">
         <v>6</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4539,13 +5112,13 @@
         <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="J8" s="2">
         <v>7</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4553,13 +5126,13 @@
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="J9" s="2">
         <v>8</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -4567,179 +5140,147 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="J10" s="2">
         <v>9</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:11">
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="J11" s="2">
         <v>10</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="E12" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
       <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="E14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="J12" s="2">
-        <v>11</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="F13" s="2">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="J13" s="2">
-        <v>12</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="F14" s="2">
-        <v>3</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J14" s="2">
-        <v>13</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="F15" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J15" s="2">
-        <v>14</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7">
+      <c r="F17" s="2">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7">
+      <c r="F18" s="2">
         <v>5</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7">
-      <c r="F17" s="2">
+      <c r="G18" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7">
+      <c r="F19" s="2">
         <v>6</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="5:7">
-      <c r="F18" s="2">
+      <c r="G19" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="F20" s="2">
         <v>7</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="5:7">
-      <c r="E20" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
       <c r="G20" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7">
       <c r="F21" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="5:7">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7">
       <c r="F22" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="5:7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7">
       <c r="F23" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="5:7">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7">
       <c r="F24" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="5:7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7">
       <c r="F25" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="5:7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7">
       <c r="F26" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="5:7">
-      <c r="F27" s="2">
-        <v>8</v>
-      </c>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7">
       <c r="G27" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="5:7">
-      <c r="F28" s="2">
-        <v>9</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
define fill up event , marker_pen test
</commit_message>
<xml_diff>
--- a/TestSteps/TestSteps diecribe.xlsx
+++ b/TestSteps/TestSteps diecribe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuia/Desktop/AppiumAutotest/TestSteps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E2788B-EB87-524E-81C1-BA82002D2568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4083A5-FA36-9B43-AAA5-74741C5BE3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="9" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="170">
   <si>
     <t>Steps</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -676,6 +676,50 @@
   </si>
   <si>
     <t>reset button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>open Marker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move bar up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move bar right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tap 'myViewBoard Display' on hotseat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>current app compare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>homepage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select pen mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select selector mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fill up left upper coner by 50 steps</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1689,27 +1733,30 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267CF906-6932-6B40-98DB-C50CCC2C8902}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
   <cols>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="45.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22">
+    <row r="1" spans="1:11">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1719,7 +1766,6 @@
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1728,6 +1774,190 @@
       </c>
       <c r="K1" s="3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="E2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="F10" s="2">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="E14" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7">
+      <c r="F17" s="2">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7">
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7">
+      <c r="F19" s="2">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="F20" s="2">
+        <v>7</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7">
+      <c r="F21" s="2">
+        <v>8</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="F22" s="2">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7">
+      <c r="F23" s="2">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="F24" s="2">
+        <v>11</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7">
+      <c r="G25" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -5025,7 +5255,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>

</xml_diff>

<commit_message>
def compare location function, marker_moving test
</commit_message>
<xml_diff>
--- a/TestSteps/TestSteps diecribe.xlsx
+++ b/TestSteps/TestSteps diecribe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuia/Desktop/AppiumAutotest/TestSteps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F08EA1C-6B71-F64A-8846-6033A94B4268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66093780-60D7-C847-A08D-9136FFCB6481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="9" xr2:uid="{17451AC4-B350-7841-B1A7-70E9EEFFBF30}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="201">
   <si>
     <t>Steps</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -777,6 +777,62 @@
   </si>
   <si>
     <t>eraser the row line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>undo &amp; redo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>undo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select delete button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>save button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>verify the file is saved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>save</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compare current app to verify the activity is closed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get element location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move bar left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move bar down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compare location different</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1790,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267CF906-6932-6B40-98DB-C50CCC2C8902}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J14"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="92" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
@@ -1806,10 +1862,14 @@
     <col min="9" max="9" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="2"/>
     <col min="11" max="11" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="10.83203125" style="2"/>
+    <col min="13" max="13" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="2"/>
+    <col min="15" max="15" width="60.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1834,8 +1894,17 @@
       <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="M1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="E2" s="4" t="s">
         <v>169</v>
       </c>
@@ -1854,8 +1923,17 @@
       <c r="K2" s="8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="M2" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N2" s="8">
+        <v>1</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="F3" s="2">
         <v>2</v>
       </c>
@@ -1868,8 +1946,14 @@
       <c r="K3" s="8" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="N3" s="8">
+        <v>2</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="F4" s="2">
         <v>3</v>
       </c>
@@ -1882,8 +1966,14 @@
       <c r="K4" s="8" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="N4" s="8">
+        <v>3</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="F5" s="2">
         <v>4</v>
       </c>
@@ -1896,8 +1986,14 @@
       <c r="K5" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="N5" s="8">
+        <v>4</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="F6" s="2">
         <v>5</v>
       </c>
@@ -1910,8 +2006,14 @@
       <c r="K6" s="8" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="N6" s="8">
+        <v>5</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="F7" s="2">
         <v>6</v>
       </c>
@@ -1924,8 +2026,14 @@
       <c r="K7" s="8" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="N7" s="8">
+        <v>6</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="F8" s="2">
         <v>7</v>
       </c>
@@ -1938,8 +2046,14 @@
       <c r="K8" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="N8" s="2">
+        <v>7</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="F9" s="2">
         <v>8</v>
       </c>
@@ -1952,8 +2066,14 @@
       <c r="K9" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="N9" s="2">
+        <v>8</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="F10" s="2">
         <v>9</v>
       </c>
@@ -1966,8 +2086,11 @@
       <c r="K10" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="O10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="F11" s="2">
         <v>10</v>
       </c>
@@ -1981,7 +2104,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:15">
       <c r="G12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1991,16 +2114,31 @@
       <c r="K12" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="M12" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="N12" s="8">
+        <v>1</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="J13" s="2">
         <v>12</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="N13" s="8">
+        <v>2</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="E14" s="4" t="s">
         <v>171</v>
       </c>
@@ -2016,8 +2154,14 @@
       <c r="K14" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="N14" s="8">
+        <v>3</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="F15" s="2">
         <v>2</v>
       </c>
@@ -2027,85 +2171,216 @@
       <c r="K15" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="N15" s="8">
+        <v>4</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="F16" s="2">
         <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="17" spans="5:7">
+      <c r="N16" s="8">
+        <v>5</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15">
       <c r="F17" s="2">
         <v>4</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="18" spans="5:7">
+      <c r="I17" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="J17" s="8">
+        <v>1</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="N17" s="8">
+        <v>6</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15">
       <c r="F18" s="2">
         <v>5</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="19" spans="5:7">
+      <c r="J18" s="8">
+        <v>2</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="N18" s="2">
+        <v>7</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15">
       <c r="F19" s="2">
         <v>6</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="20" spans="5:7">
+      <c r="J19" s="8">
+        <v>3</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="5:15">
       <c r="F20" s="2">
         <v>7</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="21" spans="5:7">
+      <c r="J20" s="8">
+        <v>4</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="5:15">
       <c r="F21" s="2">
         <v>8</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="22" spans="5:7">
+      <c r="J21" s="8">
+        <v>5</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N21" s="8">
+        <v>1</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="5:15">
       <c r="F22" s="2">
         <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="23" spans="5:7">
+      <c r="J22" s="8">
+        <v>6</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="N22" s="8">
+        <v>2</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="5:15">
       <c r="F23" s="2">
         <v>10</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="5:7">
+      <c r="J23" s="2">
+        <v>7</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="N23" s="8">
+        <v>3</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="5:15">
       <c r="F24" s="2">
         <v>11</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="25" spans="5:7">
+      <c r="J24" s="2">
+        <v>8</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N24" s="8">
+        <v>4</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="5:15">
       <c r="G25" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="5:7">
+      <c r="J25" s="2">
+        <v>9</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N25" s="8">
+        <v>5</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="5:15">
+      <c r="J26" s="2">
+        <v>10</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N26" s="8">
+        <v>6</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="5:15">
       <c r="E27" s="4" t="s">
         <v>178</v>
       </c>
@@ -2115,48 +2390,114 @@
       <c r="G27" s="8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="28" spans="5:7">
+      <c r="J27" s="2">
+        <v>11</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N27" s="8">
+        <v>7</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="5:15">
       <c r="F28" s="8">
         <v>2</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="29" spans="5:7">
+      <c r="J28" s="2">
+        <v>12</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N28" s="8">
+        <v>8</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15">
       <c r="F29" s="8">
         <v>3</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="30" spans="5:7">
+      <c r="J29" s="2">
+        <v>13</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N29" s="8">
+        <v>9</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="5:15">
       <c r="F30" s="8">
         <v>4</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="31" spans="5:7">
+      <c r="J30" s="2">
+        <v>14</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N30" s="8">
+        <v>10</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="5:15">
       <c r="F31" s="8">
         <v>5</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="32" spans="5:7">
+      <c r="J31" s="2">
+        <v>15</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N31" s="8">
+        <v>11</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="5:15">
       <c r="F32" s="8">
         <v>6</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="33" spans="6:7">
+      <c r="K32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="6:11">
       <c r="F33" s="8">
         <v>7</v>
       </c>
@@ -2164,42 +2505,136 @@
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="6:7">
+    <row r="34" spans="6:11">
       <c r="F34" s="8">
         <v>8</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="35" spans="6:7">
+      <c r="I34" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J34" s="8">
+        <v>1</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="6:11">
       <c r="F35" s="8">
         <v>9</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="36" spans="6:7">
+      <c r="J35" s="8">
+        <v>2</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11">
       <c r="F36" s="8">
         <v>10</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="37" spans="6:7">
+      <c r="J36" s="8">
+        <v>3</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11">
       <c r="F37" s="8">
         <v>11</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="38" spans="6:7">
+      <c r="J37" s="8">
+        <v>4</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11">
       <c r="F38" s="8"/>
       <c r="G38" s="8" t="s">
         <v>170</v>
+      </c>
+      <c r="J38" s="8">
+        <v>5</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11">
+      <c r="J39" s="8">
+        <v>6</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11">
+      <c r="J40" s="2">
+        <v>7</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11">
+      <c r="J41" s="2">
+        <v>8</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11">
+      <c r="J42" s="2">
+        <v>9</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11">
+      <c r="J43" s="2">
+        <v>10</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11">
+      <c r="J44" s="2">
+        <v>11</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11">
+      <c r="J45" s="2">
+        <v>12</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11">
+      <c r="K46" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>